<commit_message>
Site updated: 2019-05-31 23:45:25
</commit_message>
<xml_diff>
--- a/2019/05/31/图解辗转相除法/Squares.xlsx
+++ b/2019/05/31/图解辗转相除法/Squares.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACM\Blog\medioqrity.github.io\blog\source\_posts\图解辗转相除法\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FDBED1A-0667-42C3-8AE8-579CDE54D6AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCAE4B0-B3DB-4BE1-BB8F-60D9DD51766B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{911C5A19-6826-4913-91CB-43445023301E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -59,10 +59,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -74,14 +132,29 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -398,191 +471,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25009A0-A4B6-4ADD-8D74-B12357078F81}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L10"/>
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.609375" defaultRowHeight="24.5" customHeight="1" x14ac:dyDescent="0.8"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+    <row r="1" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="5"/>
+    </row>
+    <row r="3" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="5"/>
+    </row>
+    <row r="4" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="5"/>
+    </row>
+    <row r="5" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="5"/>
+    </row>
+    <row r="6" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="5"/>
+    </row>
+    <row r="7" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="5"/>
+    </row>
+    <row r="8" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="5"/>
+    </row>
+    <row r="9" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="5"/>
+    </row>
+    <row r="10" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="5"/>
+    </row>
+    <row r="11" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="5"/>
+    </row>
+    <row r="12" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="5"/>
+    </row>
+    <row r="13" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="5"/>
+    </row>
+    <row r="14" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="5"/>
+    </row>
+    <row r="15" spans="1:36" ht="24.5" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="6">
+        <v>21</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AJ1:AJ14"/>
+    <mergeCell ref="O15:AI15"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>